<commit_message>
Plot CRRA implied rates, compute correlation
</commit_message>
<xml_diff>
--- a/src/data/data-info.xlsx
+++ b/src/data/data-info.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\owner\Google Drive\docs\15fa\econ-thesis\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\owner\Google Drive\docs\15fa\econ-thesis\src\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="59">
   <si>
     <t>Series</t>
   </si>
@@ -186,6 +186,21 @@
   </si>
   <si>
     <t>3-month T-bill secondary market rate</t>
+  </si>
+  <si>
+    <t>cci-index</t>
+  </si>
+  <si>
+    <t>1956:Q4</t>
+  </si>
+  <si>
+    <t>Index 1947-49 = 100</t>
+  </si>
+  <si>
+    <t>Bloomberg</t>
+  </si>
+  <si>
+    <t>Continuous Commodity Index</t>
   </si>
 </sst>
 </file>
@@ -515,11 +530,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G12"/>
+  <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A13" sqref="A13"/>
+      <selection pane="bottomLeft" activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -808,6 +823,29 @@
         <v>51</v>
       </c>
     </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>58</v>
+      </c>
+      <c r="B13" t="s">
+        <v>54</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>57</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>